<commit_message>
1st general charts completed
</commit_message>
<xml_diff>
--- a/fppjan22.xlsx
+++ b/fppjan22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejaih\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD89FE72-5F43-42C7-8A08-5900DBFB901F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D6EBC3-4DA9-4A7A-84EE-0E0A0904BC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9678" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9678" uniqueCount="669">
   <si>
     <t>Progress</t>
   </si>
@@ -2083,230 +2083,7 @@
     <t>shared with their neighbors</t>
   </si>
   <si>
-    <t>Progress Progress</t>
-  </si>
-  <si>
-    <t>Duration (in seconds) Duration (in seconds)</t>
-  </si>
-  <si>
-    <t>Finished Finished</t>
-  </si>
-  <si>
-    <t>UserLanguage User Language</t>
-  </si>
-  <si>
-    <t>QID1 How satisfied are you with the food you received overall? (on a scale from extremely dissatisfied to extremely satisfied)</t>
-  </si>
-  <si>
-    <t>Q2 Have you ever received a household essentials (i.e. toilet paper/paper towels, hand sanitizer, etc.) bag?</t>
-  </si>
-  <si>
-    <t>Q4 How satisfied are you with the household essentials (i.e. toilet 
-paper/paper towels, hand sanitizer, etc.) bag?</t>
-  </si>
-  <si>
-    <t>Q5 Have you received masks from us before?</t>
-  </si>
-  <si>
-    <t>Q6 Did you and your household members wear the masks we gave you?</t>
-  </si>
-  <si>
-    <t>Q7 Were these the first masks you received?</t>
-  </si>
-  <si>
-    <t>Q9 Have you received a distribution flyer from us before?</t>
-  </si>
-  <si>
-    <t>Q10 Do you agree with the statement: I found the resources helpful.</t>
-  </si>
-  <si>
-    <t>Q11 How helpful do you find the recipes provided to you in distribution flyers?</t>
-  </si>
-  <si>
-    <t>Q65 How helpful do you find the sustainability tips (i.e., saving water and utility costs and calculating your environmental footprint) we provided to you in the summer distribution flyers?</t>
-  </si>
-  <si>
-    <t>Q66 How helpful do you find the community resources we provide to you in distribution flyers?</t>
-  </si>
-  <si>
-    <t>Q16 What information in the distribution flyer do you find the most useful? (Can pick more than 1)</t>
-  </si>
-  <si>
-    <t>Q17 What information in the distribution flyer do you find the least useful? (Can pick more than 1)</t>
-  </si>
-  <si>
-    <t>Q18 What other information would you like us to include on the distribution flyers?</t>
-  </si>
-  <si>
-    <t>Q22 Every two weeks, you get a confirmation call from us a few days before your delivery. How could we improve these confirmation calls?</t>
-  </si>
-  <si>
-    <t>Q24 In terms of our communication with you, do we contact you too much, just right, or too little?</t>
-  </si>
-  <si>
-    <t>Q26 Do you feel that you’re able to reach us easily when you have questions/concerns?</t>
-  </si>
-  <si>
-    <t>Q22 Do you have any ideas of improvements for the Fresh Produce Program? This can be as general as you would like, including mode of delivery, the produce distributed, the information on the flyers, etc.</t>
-  </si>
-  <si>
-    <t>Q24 Would you prefer a pick-up, delivery, or a hybrid model (both pick-up and delivery model) for distribution?</t>
-  </si>
-  <si>
-    <t>Q27 Would you be interested in having distribution hubs for picking up the food produce bags? These hubs would be local churches or community centers that would be determined based on proximity to your location.</t>
-  </si>
-  <si>
-    <t>Q86 Are you comfortable using all the ingredients given in the produce bag?</t>
-  </si>
-  <si>
-    <t>Q46 Which items are you unfamiliar with in the produce bag?</t>
-  </si>
-  <si>
-    <t>Q47 What produce do you wish you would have gotten in your produce bag?</t>
-  </si>
-  <si>
-    <t>Q28 How much food given in your delivery do you throw away?</t>
-  </si>
-  <si>
-    <t>Q29 Which of these categories of food was thrown away in your household in the past week? This food includes both food from FPP and not from FPP. - Selected Choice</t>
-  </si>
-  <si>
-    <t>Q29_12_TEXT Which of these categories of food was thrown away in your household in the past week? This food includes both food from FPP and not from FPP. - Other (please elaborate) - Text</t>
-  </si>
-  <si>
-    <t>Q30 How many handfuls of fresh vegetables were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q31 How many handfuls of fresh fruit were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q32 How many handfuls of canned vegetables were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q33 How many handfuls of canned fruit were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q34 How many handfuls of meat and fish were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q35 How many handfuls of dairy were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q36 How many handfuls of rice were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q37 How many handfuls of pasta were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q38 How many handfuls of beans were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q39 How many handfuls of soups were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q40 How many handfuls of chips, nuts, and other snacks were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q41 How many handfuls of "other" were disposed of in the last week?</t>
-  </si>
-  <si>
-    <t>Q42 What are the reasons food gets wasted in your home? (Can click more than one) - Selected Choice</t>
-  </si>
-  <si>
-    <t>Q42_6_TEXT What are the reasons food gets wasted in your home? (Can click more than one) - Other - Text</t>
-  </si>
-  <si>
-    <t>Q43 Do you compost at home? Composting is saving your food scraps and brown dry material like cardboard to improve soil for gardening.</t>
-  </si>
-  <si>
-    <t>Q45 Would you be interested in participating in a Fresh Produce Program composting program?</t>
-  </si>
-  <si>
-    <t>Q48 What is your COVID-19 vaccination status?</t>
-  </si>
-  <si>
-    <t>Q49 Has our program helped you to achieve any of the following:</t>
-  </si>
-  <si>
-    <t>Q50 How often do you need
-someone to help you when
-you are given information to
-read by your doctor, nurse or
-pharmacist?</t>
-  </si>
-  <si>
-    <t>Q51 When you need help, can
-you easily get hold of
-someone to assist you?</t>
-  </si>
-  <si>
-    <t>Q53 Do you need help to fill in
-official documents?</t>
-  </si>
-  <si>
-    <t>Q54 When you talk to a doctor or
-nurse, do you give them all
-the information they need to
-help you?</t>
-  </si>
-  <si>
-    <t>Q55 When you talk to a doctor or
-nurse, do you ask the
-questions you need to ask?</t>
-  </si>
-  <si>
-    <t>Q56 When you talk to a doctor or
-nurse, do you make sure
-they explain anything that
-you do not understand?</t>
-  </si>
-  <si>
-    <t>Q57 Are you someone who likes
-to find out lots of different
-information about your
-health?</t>
-  </si>
-  <si>
-    <t>Q58 How often do you think
-carefully about whether
-health information makes
-sense in your particular
-situation?</t>
-  </si>
-  <si>
-    <t>Q59 How often do you try to work
-out whether information
-about your health can be
-trusted?</t>
-  </si>
-  <si>
-    <t>Q60 Are you the sort of person
-who might question your
-doctor or nurse’s advice
-based on your own
-research?</t>
-  </si>
-  <si>
-    <t>Q62 Do you think that there
-plenty of ways to have a say
-in what the government does
-about health?</t>
-  </si>
-  <si>
-    <t>Q63 Within the last 12 months
-have you taken action to
-do something about a
-health issue that affects
-your family or
-community?</t>
-  </si>
-  <si>
-    <t>Q64 What do you think
-matters most for
-everyone’s health?</t>
-  </si>
-  <si>
-    <t>Unique ID</t>
+    <t>User ID</t>
   </si>
 </sst>
 </file>
@@ -18650,190 +18427,190 @@
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>729</v>
+        <v>668</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>668</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>669</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>670</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>671</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>672</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>673</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>674</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>675</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>676</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>677</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>678</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>679</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>680</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>681</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>682</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>683</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>684</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>685</v>
+        <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>686</v>
+        <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>687</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>688</v>
+        <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>689</v>
+        <v>18</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>690</v>
+        <v>19</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>691</v>
+        <v>21</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>692</v>
+        <v>22</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>693</v>
+        <v>23</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>694</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>695</v>
+        <v>25</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>696</v>
+        <v>26</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>697</v>
+        <v>27</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>698</v>
+        <v>28</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>699</v>
+        <v>29</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>700</v>
+        <v>30</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>701</v>
+        <v>31</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>702</v>
+        <v>32</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>703</v>
+        <v>33</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>704</v>
+        <v>34</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>705</v>
+        <v>35</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>706</v>
+        <v>36</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>707</v>
+        <v>37</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>708</v>
+        <v>38</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>709</v>
+        <v>39</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>710</v>
+        <v>40</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>711</v>
+        <v>41</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>712</v>
+        <v>42</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>713</v>
+        <v>43</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>714</v>
+        <v>44</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>715</v>
+        <v>45</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>716</v>
+        <v>46</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>717</v>
+        <v>47</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>718</v>
+        <v>48</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>719</v>
+        <v>49</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>720</v>
+        <v>50</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>721</v>
+        <v>51</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>722</v>
+        <v>52</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>723</v>
+        <v>53</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>724</v>
+        <v>54</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>725</v>
+        <v>55</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>726</v>
+        <v>56</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>727</v>
+        <v>57</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>728</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.3">

</xml_diff>